<commit_message>
viola jones modified, testing build
</commit_message>
<xml_diff>
--- a/Documents/Akurasi Train (version 1).xlsx
+++ b/Documents/Akurasi Train (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tugas-Akhir\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD276115-0103-4E62-A303-553318C7C59B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A80A7CC-E262-43E2-8366-43C88B6495AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{A5B1CD60-73A7-4347-8829-366689E28FD4}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -704,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6AFB22-F032-4202-BC26-84EC7CA8BD4B}">
   <dimension ref="A2:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>

</xml_diff>